<commit_message>
Update readme for different folder
</commit_message>
<xml_diff>
--- a/data/arcgis_climate_station_loc/Eva_Station_Satellite_In_Use.xlsx
+++ b/data/arcgis_climate_station_loc/Eva_Station_Satellite_In_Use.xlsx
@@ -1,25 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\24468\Desktop\Research\SEAS-HYDRO\Mono Lake\Mono-Evap-Pan\data\arcgis_climate_station_loc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43AB02-4271-46F0-A748-6F8772C8D396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Station" sheetId="1" r:id="rId4"/>
+    <sheet name="Station" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A6">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <t xml:space="preserve">same as the one from CDEC
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>same as the one from CDEC
 	-Yolanda Ming</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -185,35 +215,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -221,7 +255,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -231,8 +265,15 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -242,6 +283,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -256,50 +298,39 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -489,23 +520,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D12:D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="13.25"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,202 +628,202 @@
       </c>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="7">
-        <v>9800.0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>38.05</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="D2" s="5">
+        <v>9800</v>
+      </c>
+      <c r="E2" s="5">
+        <v>38.049999999999997</v>
+      </c>
+      <c r="F2" s="5">
         <v>-119.25</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="7">
-        <v>6437.0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>38.06972</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="D3" s="5">
+        <v>6437</v>
+      </c>
+      <c r="E3" s="5">
+        <v>38.069719999999997</v>
+      </c>
+      <c r="F3" s="5">
         <v>-118.9481</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="7">
-        <v>5450.0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>37.843</v>
-      </c>
-      <c r="F4" s="7">
-        <v>-118.478</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="5">
+        <v>5450</v>
+      </c>
+      <c r="E4" s="5">
+        <v>37.843000000000004</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-118.47799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7">
-        <v>2071.7</v>
-      </c>
-      <c r="E5" s="7">
-        <v>37.9567</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="D5" s="5">
+        <v>6796.9162279999991</v>
+      </c>
+      <c r="E5" s="5">
+        <v>37.956699999999998</v>
+      </c>
+      <c r="F5" s="5">
         <v>-119.1194</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="7">
-        <v>1661.2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>37.8341</v>
-      </c>
-      <c r="F6" s="7">
-        <v>-118.478</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="D6" s="5">
+        <v>5450.1314080000002</v>
+      </c>
+      <c r="E6" s="5">
+        <v>37.834099999999999</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-118.47799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="7">
-        <v>2069.9</v>
-      </c>
-      <c r="E7" s="7">
-        <v>38.2719</v>
-      </c>
-      <c r="F7" s="7">
-        <v>-119.2892</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="5">
+        <v>6791.0107160000007</v>
+      </c>
+      <c r="E7" s="5">
+        <v>38.271900000000002</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-119.28919999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="7">
-        <v>2316.5</v>
-      </c>
-      <c r="E8" s="7">
-        <v>37.745</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="D8" s="5">
+        <v>7600.0658599999997</v>
+      </c>
+      <c r="E8" s="5">
+        <v>37.744999999999997</v>
+      </c>
+      <c r="F8" s="5">
         <v>-118.983</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="7">
-        <v>2878.8</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="5">
+        <v>9444.8821920000009</v>
+      </c>
+      <c r="E9" s="5">
         <v>38.07</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>-119.23</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="7">
-        <v>2069.9</v>
-      </c>
-      <c r="E10" s="7">
-        <v>38.019663</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="D10" s="5">
+        <v>6791.0107160000007</v>
+      </c>
+      <c r="E10" s="5">
+        <v>38.019663000000001</v>
+      </c>
+      <c r="F10" s="5">
         <v>-119.166006</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="B4"/>
-    <hyperlink r:id="rId5" ref="B5"/>
-    <hyperlink r:id="rId6" ref="B6"/>
-    <hyperlink r:id="rId7" ref="B7"/>
-    <hyperlink r:id="rId8" ref="B8"/>
-    <hyperlink r:id="rId9" ref="B9"/>
-    <hyperlink r:id="rId10" ref="B10"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>